<commit_message>
+ Make game item UI for Food Item.
</commit_message>
<xml_diff>
--- a/Assets/Data/GameConfig.xlsx
+++ b/Assets/Data/GameConfig.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Avatar" sheetId="1" r:id="rId1"/>
-    <sheet name="Item" sheetId="2" r:id="rId2"/>
-    <sheet name="Weapon" sheetId="3" r:id="rId3"/>
+    <sheet name="Weapon" sheetId="4" r:id="rId2"/>
+    <sheet name="Food" sheetId="2" r:id="rId3"/>
+    <sheet name="GemStone" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="189">
   <si>
     <t>ID</t>
   </si>
@@ -254,48 +255,15 @@
     <t>Fighter</t>
   </si>
   <si>
-    <t>Đấu sĩ</t>
-  </si>
-  <si>
     <t>Mage</t>
   </si>
   <si>
-    <t>Pháp sư</t>
-  </si>
-  <si>
-    <t>Hỗ trợ</t>
-  </si>
-  <si>
     <t>Assassin</t>
   </si>
   <si>
     <t>Tank</t>
   </si>
   <si>
-    <t xml:space="preserve">Sát thủ </t>
-  </si>
-  <si>
-    <t>Sát thương bạo kích lớn, xuyên giáp lớn</t>
-  </si>
-  <si>
-    <t>Tự buff các hiệu ứng đặt biệt cho bản thân</t>
-  </si>
-  <si>
-    <t>Tăng công và thủ,sát thương máu đều các chỉ số</t>
-  </si>
-  <si>
-    <t>Tanker</t>
-  </si>
-  <si>
-    <t>Tăng HP phòng thủ , giảm sát thương</t>
-  </si>
-  <si>
-    <t>Tăng các hiệu ứng (chính xác, tốc độ, choáng, )</t>
-  </si>
-  <si>
-    <t>Bất kì nv nào cũng trang bị đk</t>
-  </si>
-  <si>
     <t>Moonlit_Firelfy</t>
   </si>
   <si>
@@ -429,13 +397,205 @@
   </si>
   <si>
     <t>STR_DRAGON_BREAD_NOODIES_USEFUL</t>
+  </si>
+  <si>
+    <t>Garnet_Gemstone</t>
+  </si>
+  <si>
+    <t>Lapis_Lazuli_Gemstone</t>
+  </si>
+  <si>
+    <t>Amethyst_Gemstone</t>
+  </si>
+  <si>
+    <t>Yellow_Jade_Gemstone</t>
+  </si>
+  <si>
+    <t>Topaz_Gemstone</t>
+  </si>
+  <si>
+    <t>Jade_Gemstone</t>
+  </si>
+  <si>
+    <t>Aquamarine_Gemstone</t>
+  </si>
+  <si>
+    <t>Garnet_Chunk</t>
+  </si>
+  <si>
+    <t>Lapis_Lazuli_Chunk</t>
+  </si>
+  <si>
+    <t>Amethyst_Chunk</t>
+  </si>
+  <si>
+    <t>Yellow_Jade_Chunk</t>
+  </si>
+  <si>
+    <t>Topaz_Chunk</t>
+  </si>
+  <si>
+    <t>Jade_Chunk</t>
+  </si>
+  <si>
+    <t>Aquamarine_Chunk</t>
+  </si>
+  <si>
+    <t>Garnet_Fragment</t>
+  </si>
+  <si>
+    <t>Lapis_Lazuli_Fragment</t>
+  </si>
+  <si>
+    <t>Amethyst_Fragment</t>
+  </si>
+  <si>
+    <t>Yellow_Jade_Fragment</t>
+  </si>
+  <si>
+    <t>Topaz_Fragment</t>
+  </si>
+  <si>
+    <t>Jade_Fragment</t>
+  </si>
+  <si>
+    <t>Aquamarine_Fragment</t>
+  </si>
+  <si>
+    <t>Garnet_Sliver</t>
+  </si>
+  <si>
+    <t>Lapis_Lazuli_Sliver</t>
+  </si>
+  <si>
+    <t>Amethyst_Sliver</t>
+  </si>
+  <si>
+    <t>Yellow_Jade_Sliver</t>
+  </si>
+  <si>
+    <t>Topaz_Sliver</t>
+  </si>
+  <si>
+    <t>Jade_Sliver</t>
+  </si>
+  <si>
+    <t>Aquamarine_Sliver</t>
+  </si>
+  <si>
+    <t>STR_AQUAMARINE_SLIVER_NAME</t>
+  </si>
+  <si>
+    <t>STR_GARNET_GEMSTONE_DES</t>
+  </si>
+  <si>
+    <t>STR_LAPIS_LAZULI_GEMSTONE_DES</t>
+  </si>
+  <si>
+    <t>STR_AMETHYST_GEMSTONE_DES</t>
+  </si>
+  <si>
+    <t>STR_YELLOW_JADE_GEMSTONE_DES</t>
+  </si>
+  <si>
+    <t>STR_TOPAZ_GEMSTONE_DES</t>
+  </si>
+  <si>
+    <t>STR_JADE_GEMSTONE_DES</t>
+  </si>
+  <si>
+    <t>STR_AQUAMARINE_GEMSTONE_DES</t>
+  </si>
+  <si>
+    <t>STR_GARNET_GEMSTONE_NAME</t>
+  </si>
+  <si>
+    <t>STR_LAPIS_LAZULI_GEMSTONE_NAME</t>
+  </si>
+  <si>
+    <t>STR_AMETHYST_GEMSTONE_NAME</t>
+  </si>
+  <si>
+    <t>STR_YELLOW_JADE_GEMSTONE_NAME</t>
+  </si>
+  <si>
+    <t>STR_TOPAZ_GEMSTONE_NAME</t>
+  </si>
+  <si>
+    <t>STR_JADE_GEMSTONE_NAME</t>
+  </si>
+  <si>
+    <t>STR_AQUAMARINE_GEMSTONE_NAME</t>
+  </si>
+  <si>
+    <t>STR_GARNET_CHUNK_NAME</t>
+  </si>
+  <si>
+    <t>STR_LAPIS_LAZULI_CHUNK_NAME</t>
+  </si>
+  <si>
+    <t>STR_AMETHYST_CHUNK_NAME</t>
+  </si>
+  <si>
+    <t>STR_YELLOW_JADE_CHUNK_NAME</t>
+  </si>
+  <si>
+    <t>STR_TOPAZ_CHUNK_NAME</t>
+  </si>
+  <si>
+    <t>STR_JADE_CHUNK_NAME</t>
+  </si>
+  <si>
+    <t>STR_AQUAMARINE_CHUNK_NAME</t>
+  </si>
+  <si>
+    <t>STR_GARNET_FRAGMENT_NAME</t>
+  </si>
+  <si>
+    <t>STR_LAPIS_LAZULI_FRAGMENT_NAME</t>
+  </si>
+  <si>
+    <t>STR_AMETHYST_FRAGMENT_NAME</t>
+  </si>
+  <si>
+    <t>STR_YELLOW_JADE_FRAGMENT_NAME</t>
+  </si>
+  <si>
+    <t>STR_TOPAZ_FRAGMENT_NAME</t>
+  </si>
+  <si>
+    <t>STR_JADE_FRAGMENT_NAME</t>
+  </si>
+  <si>
+    <t>STR_AQUAMARINE_FRAGMENT_NAME</t>
+  </si>
+  <si>
+    <t>STR_GARNET_SLIVER_NAME</t>
+  </si>
+  <si>
+    <t>STR_LAPIS_LAZULI_SLIVER_NAME</t>
+  </si>
+  <si>
+    <t>STR_AMETHYST_SLIVER_NAME</t>
+  </si>
+  <si>
+    <t>STR_YELLOW_JADE_SLIVER_NAME</t>
+  </si>
+  <si>
+    <t>STR_TOPAZ_SLIVER_NAME</t>
+  </si>
+  <si>
+    <t>STR_JADE_SLIVER_NAME</t>
+  </si>
+  <si>
+    <t>STR_GEMSTONE_USEFUL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,16 +603,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -507,6 +659,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -553,7 +711,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -985,10 +1145,422 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="6">
+        <v>683</v>
+      </c>
+      <c r="H2" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="6">
+        <v>683</v>
+      </c>
+      <c r="H3" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="6">
+        <v>683</v>
+      </c>
+      <c r="H4" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="6">
+        <v>683</v>
+      </c>
+      <c r="H5" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="6">
+        <v>683</v>
+      </c>
+      <c r="H6" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="6">
+        <v>683</v>
+      </c>
+      <c r="H7" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="6">
+        <v>683</v>
+      </c>
+      <c r="H8" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="6">
+        <v>683</v>
+      </c>
+      <c r="H9" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="6">
+        <v>683</v>
+      </c>
+      <c r="H10" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="6">
+        <v>683</v>
+      </c>
+      <c r="H11" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="6">
+        <v>683</v>
+      </c>
+      <c r="H12" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="6">
+        <v>683</v>
+      </c>
+      <c r="H13" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="6">
+        <v>683</v>
+      </c>
+      <c r="H14" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="6">
+        <v>683</v>
+      </c>
+      <c r="H15" s="6">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,7 +1573,7 @@
     <col min="18" max="18" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>27</v>
       </c>
@@ -1012,667 +1584,687 @@
         <v>25</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>28</v>
-      </c>
+      <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="M2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D3" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F3" s="6"/>
+      <c r="M3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F4" s="6"/>
+      <c r="M4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="R5" t="s">
-        <v>1</v>
-      </c>
-      <c r="S5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F5" s="6"/>
+      <c r="M5" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D6" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="R6" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="S6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F6" s="6"/>
+      <c r="M6" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="D7" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="R7" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="S7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C8" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="R8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="S8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="R9" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="R10" s="12" t="s">
-        <v>5</v>
-      </c>
+      <c r="F8" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="54.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>154</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>188</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="6">
-        <v>683</v>
-      </c>
-      <c r="H2" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>188</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="6">
-        <v>683</v>
-      </c>
-      <c r="H3" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>163</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>156</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>188</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="6">
-        <v>683</v>
-      </c>
-      <c r="H4" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>164</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="6">
-        <v>683</v>
-      </c>
-      <c r="H5" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>165</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>158</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>188</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="6">
-        <v>683</v>
-      </c>
-      <c r="H6" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>166</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="6">
-        <v>683</v>
-      </c>
-      <c r="H7" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>167</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>160</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="6">
-        <v>683</v>
-      </c>
-      <c r="H8" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>168</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>154</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>188</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F9" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="6">
-        <v>683</v>
-      </c>
-      <c r="H9" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>169</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>155</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="6">
-        <v>683</v>
-      </c>
-      <c r="H10" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>170</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>156</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G11" s="6">
-        <v>683</v>
-      </c>
-      <c r="H11" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>171</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>157</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G12" s="6">
-        <v>683</v>
-      </c>
-      <c r="H12" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>172</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" t="s">
-        <v>94</v>
-      </c>
-      <c r="G13" s="6">
-        <v>683</v>
-      </c>
-      <c r="H13" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
       <c r="B14" t="s">
-        <v>96</v>
+        <v>173</v>
       </c>
       <c r="C14" t="s">
-        <v>97</v>
+        <v>159</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>188</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F14" t="s">
-        <v>98</v>
-      </c>
-      <c r="G14" s="6">
-        <v>683</v>
-      </c>
-      <c r="H14" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="B15" t="s">
-        <v>100</v>
+        <v>174</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>160</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" t="s">
-        <v>102</v>
-      </c>
-      <c r="G15" s="6">
-        <v>683</v>
-      </c>
-      <c r="H15" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K23" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="L23" t="s">
-        <v>77</v>
-      </c>
-      <c r="M23" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K24" t="s">
-        <v>78</v>
-      </c>
-      <c r="L24" t="s">
-        <v>79</v>
-      </c>
-      <c r="M24" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K25" t="s">
-        <v>103</v>
-      </c>
-      <c r="L25" t="s">
-        <v>80</v>
-      </c>
-      <c r="M25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K26" t="s">
-        <v>81</v>
-      </c>
-      <c r="L26" t="s">
-        <v>83</v>
-      </c>
-      <c r="M26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K27" t="s">
-        <v>82</v>
-      </c>
-      <c r="L27" t="s">
-        <v>87</v>
-      </c>
-      <c r="M27" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K28" t="s">
-        <v>15</v>
-      </c>
-      <c r="M28" t="s">
-        <v>90</v>
+        <v>188</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" t="s">
+        <v>154</v>
+      </c>
+      <c r="D16" t="s">
+        <v>188</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D17" t="s">
+        <v>188</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D18" t="s">
+        <v>188</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20" t="s">
+        <v>179</v>
+      </c>
+      <c r="C20" t="s">
+        <v>158</v>
+      </c>
+      <c r="D20" t="s">
+        <v>188</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" t="s">
+        <v>159</v>
+      </c>
+      <c r="D21" t="s">
+        <v>188</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" t="s">
+        <v>181</v>
+      </c>
+      <c r="C22" t="s">
+        <v>160</v>
+      </c>
+      <c r="D22" t="s">
+        <v>188</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23" t="s">
+        <v>182</v>
+      </c>
+      <c r="C23" t="s">
+        <v>154</v>
+      </c>
+      <c r="D23" t="s">
+        <v>188</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>147</v>
+      </c>
+      <c r="B24" t="s">
+        <v>183</v>
+      </c>
+      <c r="C24" t="s">
+        <v>155</v>
+      </c>
+      <c r="D24" t="s">
+        <v>188</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>148</v>
+      </c>
+      <c r="B25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C25" t="s">
+        <v>156</v>
+      </c>
+      <c r="D25" t="s">
+        <v>188</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>149</v>
+      </c>
+      <c r="B26" t="s">
+        <v>185</v>
+      </c>
+      <c r="C26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" t="s">
+        <v>188</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" t="s">
+        <v>186</v>
+      </c>
+      <c r="C27" t="s">
+        <v>158</v>
+      </c>
+      <c r="D27" t="s">
+        <v>188</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28" t="s">
+        <v>187</v>
+      </c>
+      <c r="C28" t="s">
+        <v>159</v>
+      </c>
+      <c r="D28" t="s">
+        <v>188</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>152</v>
+      </c>
+      <c r="B29" t="s">
+        <v>153</v>
+      </c>
+      <c r="C29" t="s">
+        <v>160</v>
+      </c>
+      <c r="D29" t="s">
+        <v>188</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
+ Add Gem stone in  inventory.
</commit_message>
<xml_diff>
--- a/Assets/Data/GameConfig.xlsx
+++ b/Assets/Data/GameConfig.xlsx
@@ -604,7 +604,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -659,12 +659,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -678,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -709,9 +703,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1560,7 +1551,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,7 +1750,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,20 +1762,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>28</v>
+      <c r="E1" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
+ Add Armor in Game.
</commit_message>
<xml_diff>
--- a/Assets/Data/GameConfig.xlsx
+++ b/Assets/Data/GameConfig.xlsx
@@ -4,13 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Avatar" sheetId="1" r:id="rId1"/>
     <sheet name="Weapon" sheetId="4" r:id="rId2"/>
     <sheet name="Food" sheetId="2" r:id="rId3"/>
     <sheet name="GemStone" sheetId="5" r:id="rId4"/>
+    <sheet name="BaseArmor" sheetId="6" r:id="rId5"/>
+    <sheet name="ArmorRareModifer" sheetId="7" r:id="rId6"/>
+    <sheet name="RandomStatPool" sheetId="8" r:id="rId7"/>
+    <sheet name="ArmorSet" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="281">
   <si>
     <t>ID</t>
   </si>
@@ -589,6 +593,282 @@
   </si>
   <si>
     <t>STR_GEMSTONE_USEFUL</t>
+  </si>
+  <si>
+    <t>Armor01</t>
+  </si>
+  <si>
+    <t>Armor01_Helmet</t>
+  </si>
+  <si>
+    <t>Armor01_Chestplate</t>
+  </si>
+  <si>
+    <t>Armor01_Gloves</t>
+  </si>
+  <si>
+    <t>Armor01_Boots</t>
+  </si>
+  <si>
+    <t>Armor01_Belt</t>
+  </si>
+  <si>
+    <t>Armor01_Ring</t>
+  </si>
+  <si>
+    <t>Armor02_Helmet</t>
+  </si>
+  <si>
+    <t>Armor02_Chestplate</t>
+  </si>
+  <si>
+    <t>Armor02_Gloves</t>
+  </si>
+  <si>
+    <t>Armor02_Boots</t>
+  </si>
+  <si>
+    <t>Armor02_Belt</t>
+  </si>
+  <si>
+    <t>Armor02_Ring</t>
+  </si>
+  <si>
+    <t>Armor03_Helmet</t>
+  </si>
+  <si>
+    <t>Armor03_Chestplate</t>
+  </si>
+  <si>
+    <t>Armor03_Gloves</t>
+  </si>
+  <si>
+    <t>Armor03_Boots</t>
+  </si>
+  <si>
+    <t>Armor03_Belt</t>
+  </si>
+  <si>
+    <t>Armor03_Ring</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Helmet</t>
+  </si>
+  <si>
+    <t>Chestplate</t>
+  </si>
+  <si>
+    <t>Gloves</t>
+  </si>
+  <si>
+    <t>Boots</t>
+  </si>
+  <si>
+    <t>Belt</t>
+  </si>
+  <si>
+    <t>Ring</t>
+  </si>
+  <si>
+    <t>Armor02</t>
+  </si>
+  <si>
+    <t>Armor03</t>
+  </si>
+  <si>
+    <t>Armor04</t>
+  </si>
+  <si>
+    <t>Armor05</t>
+  </si>
+  <si>
+    <t>Armor06</t>
+  </si>
+  <si>
+    <t>Armor04_Helmet</t>
+  </si>
+  <si>
+    <t>Armor05_Helmet</t>
+  </si>
+  <si>
+    <t>Armor06_Helmet</t>
+  </si>
+  <si>
+    <t>Armor04_Boots</t>
+  </si>
+  <si>
+    <t>Armor05_Belt</t>
+  </si>
+  <si>
+    <t>Armor06_Ring</t>
+  </si>
+  <si>
+    <t>Armor04_Chestplate</t>
+  </si>
+  <si>
+    <t>Armor05_Chestplate</t>
+  </si>
+  <si>
+    <t>Armor06_Chestplate</t>
+  </si>
+  <si>
+    <t>Armor04_Gloves</t>
+  </si>
+  <si>
+    <t>Armor05_Gloves</t>
+  </si>
+  <si>
+    <t>Armor06_Gloves</t>
+  </si>
+  <si>
+    <t>Bonus</t>
+  </si>
+  <si>
+    <t>Armor05_Boots</t>
+  </si>
+  <si>
+    <t>Armor06_Boots</t>
+  </si>
+  <si>
+    <t>Armor04_Belt</t>
+  </si>
+  <si>
+    <t>Armor06_Belt</t>
+  </si>
+  <si>
+    <t>Armor04_Ring</t>
+  </si>
+  <si>
+    <t>Armor05_Ring</t>
+  </si>
+  <si>
+    <t>UnCommon</t>
+  </si>
+  <si>
+    <t>Min Substat</t>
+  </si>
+  <si>
+    <t>MaxSubStat</t>
+  </si>
+  <si>
+    <t>StatMultiplier</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.25</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>DropRare</t>
+  </si>
+  <si>
+    <t>FinalStat = BaseStat * RareMultiplier + RandomStats</t>
+  </si>
+  <si>
+    <t>SubStatID</t>
+  </si>
+  <si>
+    <t>MinValue</t>
+  </si>
+  <si>
+    <t>MaxValue</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>ATK</t>
+  </si>
+  <si>
+    <t>DEF</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>ARM_PEN</t>
+  </si>
+  <si>
+    <t>CRIT</t>
+  </si>
+  <si>
+    <t>CRIT_DMG</t>
+  </si>
+  <si>
+    <t>EFF_RES</t>
+  </si>
+  <si>
+    <t>STR_HP</t>
+  </si>
+  <si>
+    <t>STR_ATK</t>
+  </si>
+  <si>
+    <t>STR_DEF</t>
+  </si>
+  <si>
+    <t>STR_SPD</t>
+  </si>
+  <si>
+    <t>STR_ARM_PEN</t>
+  </si>
+  <si>
+    <t>STR_CRIT</t>
+  </si>
+  <si>
+    <t>STR_CRIT_DMG</t>
+  </si>
+  <si>
+    <t>STR_EFF_RES</t>
+  </si>
+  <si>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>STR_ACC</t>
+  </si>
+  <si>
+    <t>STR_ARMOR_01</t>
+  </si>
+  <si>
+    <t>STR_ARMOR_02</t>
+  </si>
+  <si>
+    <t>STR_ARMOR_03</t>
+  </si>
+  <si>
+    <t>STR_ARMOR_04</t>
+  </si>
+  <si>
+    <t>STR_ARMOR_05</t>
+  </si>
+  <si>
+    <t>STR_ARMOR_06</t>
+  </si>
+  <si>
+    <t>SetID</t>
+  </si>
+  <si>
+    <t>NumberPart</t>
+  </si>
+  <si>
+    <t>STR_ARMOR_SET_DES</t>
+  </si>
+  <si>
+    <t>SetArmor</t>
   </si>
 </sst>
 </file>
@@ -604,7 +884,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -659,6 +939,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -672,7 +970,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -705,6 +1003,12 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1749,7 +2053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -2258,4 +2562,1007 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" t="s">
+        <v>273</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B6" t="s">
+        <v>275</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B8" t="s">
+        <v>271</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B9" t="s">
+        <v>272</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B10" t="s">
+        <v>273</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B11" t="s">
+        <v>274</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B12" t="s">
+        <v>275</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13" t="s">
+        <v>276</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B14" t="s">
+        <v>271</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B15" t="s">
+        <v>272</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="B16" t="s">
+        <v>273</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="B17" t="s">
+        <v>274</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="B18" t="s">
+        <v>275</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="B19" t="s">
+        <v>276</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="B20" t="s">
+        <v>271</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="B21" t="s">
+        <v>272</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="B22" t="s">
+        <v>273</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="B23" t="s">
+        <v>274</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="B24" t="s">
+        <v>275</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="B25" t="s">
+        <v>276</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B26" t="s">
+        <v>271</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B27" t="s">
+        <v>272</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="B28" t="s">
+        <v>273</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="B29" t="s">
+        <v>274</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="B30" t="s">
+        <v>275</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="B31" t="s">
+        <v>276</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B32" t="s">
+        <v>271</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B33" t="s">
+        <v>272</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B34" t="s">
+        <v>273</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B35" t="s">
+        <v>274</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B36" t="s">
+        <v>275</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B37" t="s">
+        <v>276</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>219</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="E3" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="E4" s="6">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="E5" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" s="15">
+        <v>0</v>
+      </c>
+      <c r="D2" s="15">
+        <v>100</v>
+      </c>
+      <c r="E2" s="15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C3" s="15">
+        <v>0</v>
+      </c>
+      <c r="D3" s="15">
+        <v>100</v>
+      </c>
+      <c r="E3" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B4" t="s">
+        <v>263</v>
+      </c>
+      <c r="C4" s="15">
+        <v>0</v>
+      </c>
+      <c r="D4" s="15">
+        <v>100</v>
+      </c>
+      <c r="E4" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>256</v>
+      </c>
+      <c r="B5" t="s">
+        <v>264</v>
+      </c>
+      <c r="C5" s="15">
+        <v>0</v>
+      </c>
+      <c r="D5" s="15">
+        <v>100</v>
+      </c>
+      <c r="E5" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>257</v>
+      </c>
+      <c r="B6" t="s">
+        <v>265</v>
+      </c>
+      <c r="C6" s="15">
+        <v>0</v>
+      </c>
+      <c r="D6" s="15">
+        <v>100</v>
+      </c>
+      <c r="E6" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>258</v>
+      </c>
+      <c r="B7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C7" s="15">
+        <v>0</v>
+      </c>
+      <c r="D7" s="15">
+        <v>100</v>
+      </c>
+      <c r="E7" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>259</v>
+      </c>
+      <c r="B8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C8" s="15">
+        <v>0</v>
+      </c>
+      <c r="D8" s="15">
+        <v>100</v>
+      </c>
+      <c r="E8" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>260</v>
+      </c>
+      <c r="B9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C9" s="15">
+        <v>0</v>
+      </c>
+      <c r="D9" s="15">
+        <v>100</v>
+      </c>
+      <c r="E9" s="15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B10" t="s">
+        <v>270</v>
+      </c>
+      <c r="C10" s="15">
+        <v>0</v>
+      </c>
+      <c r="D10" s="15">
+        <v>100</v>
+      </c>
+      <c r="E10" s="15">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C2" s="15">
+        <v>4</v>
+      </c>
+      <c r="D2" s="15">
+        <v>36</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" s="15">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15">
+        <v>36</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C4" s="15">
+        <v>4</v>
+      </c>
+      <c r="D4" s="15">
+        <v>36</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C5" s="15">
+        <v>4</v>
+      </c>
+      <c r="D5" s="15">
+        <v>36</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="B6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C6" s="15">
+        <v>4</v>
+      </c>
+      <c r="D6" s="15">
+        <v>36</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C7" s="15">
+        <v>4</v>
+      </c>
+      <c r="D7" s="15">
+        <v>36</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>253</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
+ Make Character UI.
</commit_message>
<xml_diff>
--- a/Assets/Data/GameConfig.xlsx
+++ b/Assets/Data/GameConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon" sheetId="4" r:id="rId1"/>
@@ -1439,7 +1439,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2129,7 +2131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
+ Add the Upgrade Relic Panel.
</commit_message>
<xml_diff>
--- a/Assets/Data/GameConfig.xlsx
+++ b/Assets/Data/GameConfig.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="321">
   <si>
     <t>ID</t>
   </si>
@@ -84,12 +84,6 @@
   </si>
   <si>
     <t>Item</t>
-  </si>
-  <si>
-    <t>Hp</t>
-  </si>
-  <si>
-    <t>Atk</t>
   </si>
   <si>
     <t>Nimbus_Cudgel</t>
@@ -1014,7 +1008,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1099,6 +1093,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1112,7 +1112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1157,6 +1157,10 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1437,10 +1441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,7 +1456,7 @@
     <col min="6" max="6" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1469,180 +1473,222 @@
         <v>8</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>5</v>
       </c>
       <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="11">
+        <v>685</v>
+      </c>
+      <c r="H2" s="11">
+        <v>165</v>
+      </c>
+      <c r="I2" s="22">
+        <v>420</v>
+      </c>
+      <c r="J2" s="23">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="5">
-        <v>683</v>
-      </c>
-      <c r="H2" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>5</v>
       </c>
       <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="11">
+        <v>757</v>
+      </c>
+      <c r="H3" s="11">
+        <v>151</v>
+      </c>
+      <c r="I3" s="22">
+        <v>435</v>
+      </c>
+      <c r="J3" s="23">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="5">
-        <v>683</v>
-      </c>
-      <c r="H3" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="11">
+        <v>615</v>
+      </c>
+      <c r="H4" s="11">
+        <v>236</v>
+      </c>
+      <c r="I4" s="22">
+        <v>410</v>
+      </c>
+      <c r="J4" s="23">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="5">
-        <v>683</v>
-      </c>
-      <c r="H4" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="11">
+        <v>458</v>
+      </c>
+      <c r="H5" s="11">
+        <v>78</v>
+      </c>
+      <c r="I5" s="22">
+        <v>210</v>
+      </c>
+      <c r="J5" s="23">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="5">
-        <v>683</v>
-      </c>
-      <c r="H5" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
         <v>36</v>
       </c>
-      <c r="B6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
       <c r="D6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>5</v>
       </c>
       <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="11">
+        <v>683</v>
+      </c>
+      <c r="H6" s="11">
+        <v>90</v>
+      </c>
+      <c r="I6" s="22">
+        <v>450</v>
+      </c>
+      <c r="J6" s="23">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="5">
-        <v>683</v>
-      </c>
-      <c r="H6" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
         <v>40</v>
       </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="11">
+        <v>458</v>
+      </c>
+      <c r="H7" s="11">
+        <v>74</v>
+      </c>
+      <c r="I7" s="22">
+        <v>210</v>
+      </c>
+      <c r="J7" s="23">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="5">
-        <v>683</v>
-      </c>
-      <c r="H7" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C8" t="s">
         <v>44</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -1651,50 +1697,62 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="11">
+        <v>256</v>
+      </c>
+      <c r="H8" s="11">
+        <v>53</v>
+      </c>
+      <c r="I8" s="22">
+        <v>130</v>
+      </c>
+      <c r="J8" s="23">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="5">
-        <v>683</v>
-      </c>
-      <c r="H8" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9" t="s">
         <v>48</v>
       </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" t="s">
-        <v>50</v>
-      </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>4</v>
       </c>
       <c r="F9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="11">
+        <v>560</v>
+      </c>
+      <c r="H9" s="11">
+        <v>143</v>
+      </c>
+      <c r="I9" s="22">
+        <v>360</v>
+      </c>
+      <c r="J9" s="23">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="5">
-        <v>683</v>
-      </c>
-      <c r="H9" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
         <v>52</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -1703,24 +1761,30 @@
         <v>3</v>
       </c>
       <c r="F10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="11">
+        <v>365</v>
+      </c>
+      <c r="H10" s="11">
+        <v>64</v>
+      </c>
+      <c r="I10" s="22">
+        <v>180</v>
+      </c>
+      <c r="J10" s="23">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="5">
-        <v>683</v>
-      </c>
-      <c r="H10" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C11" t="s">
         <v>56</v>
-      </c>
-      <c r="B11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" t="s">
-        <v>58</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -1729,117 +1793,147 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="11">
+        <v>256</v>
+      </c>
+      <c r="H11" s="11">
+        <v>53</v>
+      </c>
+      <c r="I11" s="22">
+        <v>130</v>
+      </c>
+      <c r="J11" s="23">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="5">
-        <v>683</v>
-      </c>
-      <c r="H11" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" t="s">
         <v>60</v>
       </c>
-      <c r="B12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" t="s">
-        <v>62</v>
-      </c>
       <c r="D12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="11">
+        <v>365</v>
+      </c>
+      <c r="H12" s="11">
+        <v>64</v>
+      </c>
+      <c r="I12" s="22">
+        <v>190</v>
+      </c>
+      <c r="J12" s="23">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
         <v>63</v>
-      </c>
-      <c r="G12" s="5">
-        <v>683</v>
-      </c>
-      <c r="H12" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" t="s">
-        <v>65</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>5</v>
       </c>
       <c r="F13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="11">
+        <v>627</v>
+      </c>
+      <c r="H13" s="11">
+        <v>134</v>
+      </c>
+      <c r="I13" s="22">
+        <v>380</v>
+      </c>
+      <c r="J13" s="23">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
         <v>70</v>
       </c>
-      <c r="G13" s="5">
-        <v>683</v>
-      </c>
-      <c r="H13" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C14" t="s">
         <v>71</v>
       </c>
-      <c r="B14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" t="s">
-        <v>73</v>
-      </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>4</v>
       </c>
       <c r="F14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="11">
+        <v>560</v>
+      </c>
+      <c r="H14" s="11">
+        <v>140</v>
+      </c>
+      <c r="I14" s="22">
+        <v>360</v>
+      </c>
+      <c r="J14" s="23">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" t="s">
         <v>74</v>
       </c>
-      <c r="G14" s="5">
-        <v>683</v>
-      </c>
-      <c r="H14" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>77</v>
-      </c>
-      <c r="D15" t="s">
-        <v>79</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15" s="5">
+        <v>76</v>
+      </c>
+      <c r="G15" s="11">
         <v>683</v>
       </c>
-      <c r="H15" s="5">
-        <v>70</v>
+      <c r="H15" s="11">
+        <v>110</v>
+      </c>
+      <c r="I15" s="22">
+        <v>395</v>
+      </c>
+      <c r="J15" s="23">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -1883,82 +1977,82 @@
         <v>16</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>317</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1966,160 +2060,160 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E9" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F9" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G9" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F11" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G11" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -2148,13 +2242,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>320</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>322</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>8</v>
@@ -2163,13 +2257,13 @@
         <v>16</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>240</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>242</v>
       </c>
       <c r="J1" s="14"/>
       <c r="K1" s="14"/>
@@ -2178,7 +2272,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B2" s="14">
         <v>375</v>
@@ -2193,7 +2287,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G2" s="14">
         <v>3750</v>
@@ -2223,7 +2317,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B3" s="14">
         <v>175</v>
@@ -2238,7 +2332,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G3" s="14">
         <v>2500</v>
@@ -2268,7 +2362,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B4" s="14">
         <v>350</v>
@@ -2283,7 +2377,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G4" s="14">
         <v>3900</v>
@@ -2317,7 +2411,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G5" s="14">
         <v>2900</v>
@@ -2336,7 +2430,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B6" s="14">
         <v>234</v>
@@ -2351,7 +2445,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G6" s="14">
         <v>29302</v>
@@ -2370,7 +2464,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B7" s="14">
         <v>238</v>
@@ -2385,7 +2479,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G7" s="14">
         <v>2650</v>
@@ -2404,7 +2498,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B8" s="14">
         <v>220</v>
@@ -2419,7 +2513,7 @@
         <v>10</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G8" s="14">
         <v>2750</v>
@@ -2438,7 +2532,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B9" s="14">
         <v>425</v>
@@ -2453,7 +2547,7 @@
         <v>11</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G9" s="14">
         <v>4250</v>
@@ -2472,7 +2566,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B10" s="14">
         <v>370</v>
@@ -2487,7 +2581,7 @@
         <v>11</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G10" s="14">
         <v>3700</v>
@@ -2506,7 +2600,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B11" s="14">
         <v>300</v>
@@ -2521,7 +2615,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G11" s="14">
         <v>3000</v>
@@ -2570,42 +2664,42 @@
         <v>16</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>243</v>
-      </c>
       <c r="H1" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>299</v>
-      </c>
       <c r="K1" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D2" s="14">
         <v>3750</v>
@@ -2637,13 +2731,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D3" s="14">
         <v>2500</v>
@@ -2675,13 +2769,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D4" s="14">
         <v>3900</v>
@@ -2719,7 +2813,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D5" s="14">
         <v>2900</v>
@@ -2751,13 +2845,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D6" s="14">
         <v>2930</v>
@@ -2789,13 +2883,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D7" s="14">
         <v>2650</v>
@@ -2827,13 +2921,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D8" s="14">
         <v>2750</v>
@@ -2865,13 +2959,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D9" s="14">
         <v>4250</v>
@@ -2903,13 +2997,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D10" s="14">
         <v>3700</v>
@@ -2941,13 +3035,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D11" s="14">
         <v>3000</v>
@@ -3011,7 +3105,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>8</v>
@@ -3022,21 +3116,21 @@
         <v>1</v>
       </c>
       <c r="N1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>86</v>
-      </c>
-      <c r="C2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" t="s">
-        <v>88</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>4</v>
@@ -3052,16 +3146,16 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
         <v>89</v>
       </c>
-      <c r="B3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" t="s">
-        <v>91</v>
-      </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>3</v>
@@ -3071,21 +3165,21 @@
         <v>3</v>
       </c>
       <c r="N3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" t="s">
         <v>92</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>93</v>
-      </c>
-      <c r="C4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" t="s">
-        <v>95</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>2</v>
@@ -3095,21 +3189,21 @@
         <v>8</v>
       </c>
       <c r="N4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
         <v>96</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>97</v>
-      </c>
-      <c r="C5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" t="s">
-        <v>99</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>2</v>
@@ -3121,16 +3215,16 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" t="s">
         <v>100</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>101</v>
-      </c>
-      <c r="C6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" t="s">
-        <v>103</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>5</v>
@@ -3142,16 +3236,16 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" t="s">
         <v>104</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>105</v>
-      </c>
-      <c r="C7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7" t="s">
-        <v>107</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>8</v>
@@ -3160,16 +3254,16 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
         <v>108</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>109</v>
-      </c>
-      <c r="C8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" t="s">
-        <v>111</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>5</v>
@@ -3208,7 +3302,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>8</v>
@@ -3216,16 +3310,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>5</v>
@@ -3233,16 +3327,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>5</v>
@@ -3250,16 +3344,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>5</v>
@@ -3267,16 +3361,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>5</v>
@@ -3284,16 +3378,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>5</v>
@@ -3301,16 +3395,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>5</v>
@@ -3318,16 +3412,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>5</v>
@@ -3335,16 +3429,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>4</v>
@@ -3352,16 +3446,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>4</v>
@@ -3369,16 +3463,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>4</v>
@@ -3386,16 +3480,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>4</v>
@@ -3403,16 +3497,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>4</v>
@@ -3420,16 +3514,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>4</v>
@@ -3437,16 +3531,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>4</v>
@@ -3454,16 +3548,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>8</v>
@@ -3471,16 +3565,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D17" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>8</v>
@@ -3488,16 +3582,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>8</v>
@@ -3505,16 +3599,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>8</v>
@@ -3522,16 +3616,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D20" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>8</v>
@@ -3539,16 +3633,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C21" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>8</v>
@@ -3556,16 +3650,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C22" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>8</v>
@@ -3573,16 +3667,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>3</v>
@@ -3590,16 +3684,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>3</v>
@@ -3607,16 +3701,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B25" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C25" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>3</v>
@@ -3624,16 +3718,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>3</v>
@@ -3641,16 +3735,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B27" t="s">
+        <v>171</v>
+      </c>
+      <c r="C27" t="s">
+        <v>143</v>
+      </c>
+      <c r="D27" t="s">
         <v>173</v>
-      </c>
-      <c r="C27" t="s">
-        <v>145</v>
-      </c>
-      <c r="D27" t="s">
-        <v>175</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>3</v>
@@ -3658,16 +3752,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B28" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C28" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>3</v>
@@ -3675,16 +3769,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B29" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D29" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>3</v>
@@ -3724,27 +3818,27 @@
         <v>13</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>3</v>
@@ -3755,16 +3849,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>8</v>
@@ -3775,16 +3869,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C4" t="s">
         <v>307</v>
       </c>
-      <c r="C4" t="s">
-        <v>309</v>
-      </c>
       <c r="D4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>4</v>
@@ -3795,16 +3889,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C5" t="s">
+        <v>307</v>
+      </c>
+      <c r="D5" t="s">
         <v>308</v>
-      </c>
-      <c r="C5" t="s">
-        <v>309</v>
-      </c>
-      <c r="D5" t="s">
-        <v>310</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>5</v>
@@ -3846,514 +3940,514 @@
         <v>14</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B12" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B15" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B17" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B18" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B19" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B20" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B21" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B22" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B24" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B25" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B26" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B27" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C27" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="D27" s="14" t="s">
         <v>200</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B28" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B29" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B30" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B31" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B32" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B33" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B34" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C34" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="D34" s="14" t="s">
         <v>201</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B35" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B36" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B37" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -4383,16 +4477,16 @@
         <v>15</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>229</v>
-      </c>
       <c r="E1" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4414,7 +4508,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -4423,7 +4517,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E3" s="5">
         <v>25</v>
@@ -4440,13 +4534,13 @@
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E4" s="5">
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4460,7 +4554,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E5" s="5">
         <v>4</v>
@@ -4477,7 +4571,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
@@ -4507,27 +4601,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>237</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C2" s="14">
         <v>0</v>
@@ -4541,10 +4635,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C3" s="14">
         <v>0</v>
@@ -4558,10 +4652,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C4" s="14">
         <v>0</v>
@@ -4575,10 +4669,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C5" s="14">
         <v>0</v>
@@ -4592,10 +4686,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C6" s="14">
         <v>0</v>
@@ -4609,10 +4703,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C7" s="14">
         <v>0</v>
@@ -4626,10 +4720,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C8" s="14">
         <v>0</v>
@@ -4643,10 +4737,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C9" s="14">
         <v>0</v>
@@ -4660,10 +4754,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C10" s="14">
         <v>0</v>
@@ -4699,27 +4793,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C2" s="14">
         <v>4</v>
@@ -4728,15 +4822,15 @@
         <v>36</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C3" s="14">
         <v>4</v>
@@ -4745,15 +4839,15 @@
         <v>36</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C4" s="14">
         <v>4</v>
@@ -4762,15 +4856,15 @@
         <v>36</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C5" s="14">
         <v>4</v>
@@ -4779,15 +4873,15 @@
         <v>36</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C6" s="14">
         <v>4</v>
@@ -4796,15 +4890,15 @@
         <v>36</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C7" s="14">
         <v>4</v>
@@ -4813,7 +4907,7 @@
         <v>36</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -4853,13 +4947,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>5</v>
@@ -4867,13 +4961,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
@@ -4881,13 +4975,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" t="s">
         <v>274</v>
-      </c>
-      <c r="C4" t="s">
-        <v>276</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>4</v>
@@ -4895,13 +4989,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>8</v>
@@ -4909,13 +5003,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>8</v>
@@ -4923,13 +5017,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C7" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>5</v>
@@ -4937,13 +5031,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>2</v>
@@ -4951,13 +5045,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>5</v>
@@ -4965,13 +5059,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>5</v>
@@ -4979,13 +5073,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C11" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
+ Fix UI bugs in Character Scene.
</commit_message>
<xml_diff>
--- a/Assets/Data/GameConfig.xlsx
+++ b/Assets/Data/GameConfig.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon" sheetId="4" r:id="rId1"/>
     <sheet name="Food" sheetId="2" r:id="rId2"/>
-    <sheet name="GemStone" sheetId="5" r:id="rId3"/>
-    <sheet name="Exp" sheetId="13" r:id="rId4"/>
-    <sheet name="BaseArmor" sheetId="6" r:id="rId5"/>
-    <sheet name="ArmorRareModifer" sheetId="7" r:id="rId6"/>
-    <sheet name="RandomStatPool" sheetId="8" r:id="rId7"/>
-    <sheet name="ArmorSet" sheetId="9" r:id="rId8"/>
-    <sheet name="Shard" sheetId="10" r:id="rId9"/>
-    <sheet name="Character" sheetId="12" r:id="rId10"/>
-    <sheet name="CharacterUpgrade" sheetId="14" r:id="rId11"/>
-    <sheet name="CharacterStat" sheetId="15" r:id="rId12"/>
+    <sheet name="Items" sheetId="16" r:id="rId3"/>
+    <sheet name="GemStone" sheetId="5" r:id="rId4"/>
+    <sheet name="Exp" sheetId="13" r:id="rId5"/>
+    <sheet name="BaseArmor" sheetId="6" r:id="rId6"/>
+    <sheet name="ArmorRareModifer" sheetId="7" r:id="rId7"/>
+    <sheet name="RandomStatPool" sheetId="8" r:id="rId8"/>
+    <sheet name="ArmorSet" sheetId="9" r:id="rId9"/>
+    <sheet name="Shard" sheetId="10" r:id="rId10"/>
+    <sheet name="Character" sheetId="12" r:id="rId11"/>
+    <sheet name="CharacterUpgrade" sheetId="14" r:id="rId12"/>
+    <sheet name="CharacterStat" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="337">
   <si>
     <t>ID</t>
   </si>
@@ -758,18 +759,9 @@
     <t>SPD</t>
   </si>
   <si>
-    <t>ARM_PEN</t>
-  </si>
-  <si>
-    <t>CRIT</t>
-  </si>
-  <si>
     <t>CRIT_DMG</t>
   </si>
   <si>
-    <t>EFF_RES</t>
-  </si>
-  <si>
     <t>STR_HP</t>
   </si>
   <si>
@@ -782,24 +774,9 @@
     <t>STR_SPD</t>
   </si>
   <si>
-    <t>STR_ARM_PEN</t>
-  </si>
-  <si>
-    <t>STR_CRIT</t>
-  </si>
-  <si>
     <t>STR_CRIT_DMG</t>
   </si>
   <si>
-    <t>STR_EFF_RES</t>
-  </si>
-  <si>
-    <t>ACC</t>
-  </si>
-  <si>
-    <t>STR_ACC</t>
-  </si>
-  <si>
     <t>STR_ARMOR_01</t>
   </si>
   <si>
@@ -993,6 +970,78 @@
   </si>
   <si>
     <t>GrowthDEF</t>
+  </si>
+  <si>
+    <t>STR_PENETRATION</t>
+  </si>
+  <si>
+    <t>STR_CRIT_DMG_RES</t>
+  </si>
+  <si>
+    <t>PEN</t>
+  </si>
+  <si>
+    <t>CRIT_DMG_RES</t>
+  </si>
+  <si>
+    <t>DEF_SHRED</t>
+  </si>
+  <si>
+    <t>STR_DEF_SHRED</t>
+  </si>
+  <si>
+    <t>CRIT_RATE</t>
+  </si>
+  <si>
+    <t>STR_CRIT_RATE</t>
+  </si>
+  <si>
+    <t>Coin</t>
+  </si>
+  <si>
+    <t>STR_COIN</t>
+  </si>
+  <si>
+    <t>STR_RELIC_ESSENCE</t>
+  </si>
+  <si>
+    <t>STR_ARMOR_PRIMORITE</t>
+  </si>
+  <si>
+    <t>STR_COIN_DES</t>
+  </si>
+  <si>
+    <t>STR_RELIC_ESSENCE_DES</t>
+  </si>
+  <si>
+    <t>STR_ARMOR_PRIMORITE_DES</t>
+  </si>
+  <si>
+    <t>STR_COIN_USE</t>
+  </si>
+  <si>
+    <t>STR_RELIC_ESSENCE_USE</t>
+  </si>
+  <si>
+    <t>STR_ARMOR_PRIMORITE_USE</t>
+  </si>
+  <si>
+    <t>Jade</t>
+  </si>
+  <si>
+    <t>STR_JADE</t>
+  </si>
+  <si>
+    <t>STR_JADE_DES</t>
+  </si>
+  <si>
+    <t>STR_JADE_USE</t>
+  </si>
+  <si>
+    <t>RelicEssence</t>
+  </si>
+  <si>
+    <t>ArmorPrimorite</t>
   </si>
 </sst>
 </file>
@@ -1443,7 +1492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -1482,10 +1531,10 @@
         <v>239</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1627,7 +1676,7 @@
         <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>5</v>
@@ -1819,7 +1868,7 @@
         <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>3</v>
@@ -1942,6 +1991,181 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B4" t="s">
+        <v>264</v>
+      </c>
+      <c r="C4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B5" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" t="s">
+        <v>266</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>268</v>
+      </c>
+      <c r="B6" t="s">
+        <v>267</v>
+      </c>
+      <c r="C6" t="s">
+        <v>266</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C7" t="s">
+        <v>266</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>278</v>
+      </c>
+      <c r="B8" t="s">
+        <v>271</v>
+      </c>
+      <c r="C8" t="s">
+        <v>266</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" t="s">
+        <v>266</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>274</v>
+      </c>
+      <c r="B10" t="s">
+        <v>275</v>
+      </c>
+      <c r="C10" t="s">
+        <v>266</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>276</v>
+      </c>
+      <c r="B11" t="s">
+        <v>277</v>
+      </c>
+      <c r="C11" t="s">
+        <v>266</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -1977,21 +2201,21 @@
         <v>16</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>11</v>
@@ -2000,21 +2224,21 @@
         <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="F2" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="G2" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B3" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>9</v>
@@ -2023,36 +2247,36 @@
         <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="F3" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="G3" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B4" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="E4" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="F4" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="G4" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2060,7 +2284,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>10</v>
@@ -2069,21 +2293,21 @@
         <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="F5" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="G5" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B6" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>10</v>
@@ -2092,21 +2316,21 @@
         <v>77</v>
       </c>
       <c r="E6" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="F6" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="G6" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B7" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>12</v>
@@ -2115,67 +2339,67 @@
         <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="F7" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="G7" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="B8" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="E8" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="F8" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="G8" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B9" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="E9" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="F9" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="G9" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="B10" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>11</v>
@@ -2184,21 +2408,21 @@
         <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="F10" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="G10" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B11" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>11</v>
@@ -2207,13 +2431,13 @@
         <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="F11" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="G11" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -2221,7 +2445,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
@@ -2242,13 +2466,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>8</v>
@@ -2272,7 +2496,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B2" s="14">
         <v>375</v>
@@ -2317,7 +2541,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B3" s="14">
         <v>175</v>
@@ -2362,7 +2586,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B4" s="14">
         <v>350</v>
@@ -2377,7 +2601,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="G4" s="14">
         <v>3900</v>
@@ -2430,7 +2654,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B6" s="14">
         <v>234</v>
@@ -2464,7 +2688,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B7" s="14">
         <v>238</v>
@@ -2498,7 +2722,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="B8" s="14">
         <v>220</v>
@@ -2513,7 +2737,7 @@
         <v>10</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="G8" s="14">
         <v>2750</v>
@@ -2532,7 +2756,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B9" s="14">
         <v>425</v>
@@ -2547,7 +2771,7 @@
         <v>11</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="G9" s="14">
         <v>4250</v>
@@ -2566,7 +2790,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="B10" s="14">
         <v>370</v>
@@ -2600,7 +2824,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B11" s="14">
         <v>300</v>
@@ -2638,7 +2862,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
@@ -2676,24 +2900,24 @@
         <v>241</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>11</v>
@@ -2731,7 +2955,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>9</v>
@@ -2769,13 +2993,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D4" s="14">
         <v>3900</v>
@@ -2845,7 +3069,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>10</v>
@@ -2883,7 +3107,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>12</v>
@@ -2921,13 +3145,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="D8" s="14">
         <v>2750</v>
@@ -2959,13 +3183,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D9" s="14">
         <v>4250</v>
@@ -2997,13 +3221,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D10" s="14">
         <v>3700</v>
@@ -3035,7 +3259,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>11</v>
@@ -3081,7 +3305,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3277,11 +3501,115 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>335</v>
+      </c>
+      <c r="B4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C4" t="s">
+        <v>326</v>
+      </c>
+      <c r="D4" t="s">
+        <v>329</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>336</v>
+      </c>
+      <c r="B5" t="s">
+        <v>324</v>
+      </c>
+      <c r="C5" t="s">
+        <v>327</v>
+      </c>
+      <c r="D5" t="s">
+        <v>330</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3790,7 +4118,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -3824,21 +4152,21 @@
         <v>8</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C2" t="s">
         <v>299</v>
       </c>
-      <c r="B2" t="s">
-        <v>303</v>
-      </c>
-      <c r="C2" t="s">
-        <v>307</v>
-      </c>
       <c r="D2" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>3</v>
@@ -3849,16 +4177,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B3" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="C3" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="D3" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>8</v>
@@ -3869,16 +4197,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D4" t="s">
         <v>300</v>
-      </c>
-      <c r="B4" t="s">
-        <v>305</v>
-      </c>
-      <c r="C4" t="s">
-        <v>307</v>
-      </c>
-      <c r="D4" t="s">
-        <v>308</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>4</v>
@@ -3889,16 +4217,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B5" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="C5" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="D5" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>5</v>
@@ -3912,12 +4240,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3943,7 +4271,7 @@
         <v>193</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3951,7 +4279,7 @@
         <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>194</v>
@@ -3965,7 +4293,7 @@
         <v>181</v>
       </c>
       <c r="B3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>194</v>
@@ -3979,7 +4307,7 @@
         <v>187</v>
       </c>
       <c r="B4" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>194</v>
@@ -3993,7 +4321,7 @@
         <v>205</v>
       </c>
       <c r="B5" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>194</v>
@@ -4007,7 +4335,7 @@
         <v>206</v>
       </c>
       <c r="B6" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>194</v>
@@ -4021,7 +4349,7 @@
         <v>207</v>
       </c>
       <c r="B7" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>194</v>
@@ -4035,7 +4363,7 @@
         <v>176</v>
       </c>
       <c r="B8" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>195</v>
@@ -4049,7 +4377,7 @@
         <v>182</v>
       </c>
       <c r="B9" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>195</v>
@@ -4063,7 +4391,7 @@
         <v>188</v>
       </c>
       <c r="B10" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>195</v>
@@ -4077,7 +4405,7 @@
         <v>211</v>
       </c>
       <c r="B11" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>195</v>
@@ -4091,7 +4419,7 @@
         <v>212</v>
       </c>
       <c r="B12" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>195</v>
@@ -4105,7 +4433,7 @@
         <v>213</v>
       </c>
       <c r="B13" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>195</v>
@@ -4119,7 +4447,7 @@
         <v>177</v>
       </c>
       <c r="B14" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>196</v>
@@ -4133,7 +4461,7 @@
         <v>183</v>
       </c>
       <c r="B15" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>196</v>
@@ -4147,7 +4475,7 @@
         <v>189</v>
       </c>
       <c r="B16" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>196</v>
@@ -4161,7 +4489,7 @@
         <v>214</v>
       </c>
       <c r="B17" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>196</v>
@@ -4175,7 +4503,7 @@
         <v>215</v>
       </c>
       <c r="B18" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>196</v>
@@ -4189,7 +4517,7 @@
         <v>216</v>
       </c>
       <c r="B19" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>196</v>
@@ -4203,7 +4531,7 @@
         <v>178</v>
       </c>
       <c r="B20" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>197</v>
@@ -4217,7 +4545,7 @@
         <v>184</v>
       </c>
       <c r="B21" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>197</v>
@@ -4231,7 +4559,7 @@
         <v>190</v>
       </c>
       <c r="B22" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>197</v>
@@ -4245,7 +4573,7 @@
         <v>208</v>
       </c>
       <c r="B23" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>197</v>
@@ -4259,7 +4587,7 @@
         <v>218</v>
       </c>
       <c r="B24" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>197</v>
@@ -4273,7 +4601,7 @@
         <v>219</v>
       </c>
       <c r="B25" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>197</v>
@@ -4287,7 +4615,7 @@
         <v>179</v>
       </c>
       <c r="B26" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>198</v>
@@ -4301,7 +4629,7 @@
         <v>185</v>
       </c>
       <c r="B27" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>198</v>
@@ -4315,7 +4643,7 @@
         <v>191</v>
       </c>
       <c r="B28" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>198</v>
@@ -4329,7 +4657,7 @@
         <v>220</v>
       </c>
       <c r="B29" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>198</v>
@@ -4343,7 +4671,7 @@
         <v>209</v>
       </c>
       <c r="B30" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>198</v>
@@ -4357,7 +4685,7 @@
         <v>221</v>
       </c>
       <c r="B31" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>198</v>
@@ -4371,7 +4699,7 @@
         <v>180</v>
       </c>
       <c r="B32" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>199</v>
@@ -4385,7 +4713,7 @@
         <v>186</v>
       </c>
       <c r="B33" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>199</v>
@@ -4399,7 +4727,7 @@
         <v>192</v>
       </c>
       <c r="B34" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>199</v>
@@ -4413,7 +4741,7 @@
         <v>222</v>
       </c>
       <c r="B35" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>199</v>
@@ -4427,7 +4755,7 @@
         <v>223</v>
       </c>
       <c r="B36" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>199</v>
@@ -4441,7 +4769,7 @@
         <v>210</v>
       </c>
       <c r="B37" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>199</v>
@@ -4455,7 +4783,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -4582,12 +4910,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4621,7 +4949,7 @@
         <v>238</v>
       </c>
       <c r="B2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C2" s="14">
         <v>0</v>
@@ -4638,7 +4966,7 @@
         <v>239</v>
       </c>
       <c r="B3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C3" s="14">
         <v>0</v>
@@ -4655,7 +4983,7 @@
         <v>240</v>
       </c>
       <c r="B4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C4" s="14">
         <v>0</v>
@@ -4672,7 +5000,7 @@
         <v>241</v>
       </c>
       <c r="B5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C5" s="14">
         <v>0</v>
@@ -4686,10 +5014,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>242</v>
+        <v>317</v>
       </c>
       <c r="B6" t="s">
-        <v>250</v>
+        <v>318</v>
       </c>
       <c r="C6" s="14">
         <v>0</v>
@@ -4703,10 +5031,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>243</v>
+        <v>319</v>
       </c>
       <c r="B7" t="s">
-        <v>251</v>
+        <v>320</v>
       </c>
       <c r="C7" s="14">
         <v>0</v>
@@ -4720,10 +5048,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B8" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C8" s="14">
         <v>0</v>
@@ -4737,10 +5065,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>245</v>
+        <v>315</v>
       </c>
       <c r="B9" t="s">
-        <v>253</v>
+        <v>313</v>
       </c>
       <c r="C9" s="14">
         <v>0</v>
@@ -4754,10 +5082,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>254</v>
+        <v>316</v>
       </c>
       <c r="B10" t="s">
-        <v>255</v>
+        <v>314</v>
       </c>
       <c r="C10" s="14">
         <v>0</v>
@@ -4774,7 +5102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -4793,13 +5121,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>217</v>
@@ -4813,7 +5141,7 @@
         <v>174</v>
       </c>
       <c r="B2" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C2" s="14">
         <v>4</v>
@@ -4830,7 +5158,7 @@
         <v>200</v>
       </c>
       <c r="B3" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C3" s="14">
         <v>4</v>
@@ -4847,7 +5175,7 @@
         <v>201</v>
       </c>
       <c r="B4" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C4" s="14">
         <v>4</v>
@@ -4864,7 +5192,7 @@
         <v>202</v>
       </c>
       <c r="B5" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C5" s="14">
         <v>4</v>
@@ -4881,7 +5209,7 @@
         <v>203</v>
       </c>
       <c r="B6" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C6" s="14">
         <v>4</v>
@@ -4898,7 +5226,7 @@
         <v>204</v>
       </c>
       <c r="B7" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C7" s="14">
         <v>4</v>
@@ -4908,181 +5236,6 @@
       </c>
       <c r="E7" s="14" t="s">
         <v>238</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>266</v>
-      </c>
-      <c r="B2" t="s">
-        <v>270</v>
-      </c>
-      <c r="C2" t="s">
-        <v>274</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>267</v>
-      </c>
-      <c r="B3" t="s">
-        <v>271</v>
-      </c>
-      <c r="C3" t="s">
-        <v>274</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>268</v>
-      </c>
-      <c r="B4" t="s">
-        <v>272</v>
-      </c>
-      <c r="C4" t="s">
-        <v>274</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>269</v>
-      </c>
-      <c r="B5" t="s">
-        <v>273</v>
-      </c>
-      <c r="C5" t="s">
-        <v>274</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>276</v>
-      </c>
-      <c r="B6" t="s">
-        <v>275</v>
-      </c>
-      <c r="C6" t="s">
-        <v>274</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>277</v>
-      </c>
-      <c r="B7" t="s">
-        <v>278</v>
-      </c>
-      <c r="C7" t="s">
-        <v>274</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>286</v>
-      </c>
-      <c r="B8" t="s">
-        <v>279</v>
-      </c>
-      <c r="C8" t="s">
-        <v>274</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>280</v>
-      </c>
-      <c r="B9" t="s">
-        <v>281</v>
-      </c>
-      <c r="C9" t="s">
-        <v>274</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>282</v>
-      </c>
-      <c r="B10" t="s">
-        <v>283</v>
-      </c>
-      <c r="C10" t="s">
-        <v>274</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>284</v>
-      </c>
-      <c r="B11" t="s">
-        <v>285</v>
-      </c>
-      <c r="C11" t="s">
-        <v>274</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ Add Animation and HeathBar for one character.
</commit_message>
<xml_diff>
--- a/Assets/Data/GameConfig.xlsx
+++ b/Assets/Data/GameConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="8" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon" sheetId="4" r:id="rId1"/>
@@ -20,6 +20,10 @@
     <sheet name="Character" sheetId="12" r:id="rId11"/>
     <sheet name="CharacterUpgrade" sheetId="14" r:id="rId12"/>
     <sheet name="CharacterStat" sheetId="15" r:id="rId13"/>
+    <sheet name="Skill" sheetId="17" r:id="rId14"/>
+    <sheet name="SkillLevel" sheetId="18" r:id="rId15"/>
+    <sheet name="Effect" sheetId="19" r:id="rId16"/>
+    <sheet name="Passive" sheetId="20" r:id="rId17"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="417">
   <si>
     <t>ID</t>
   </si>
@@ -1042,6 +1046,246 @@
   </si>
   <si>
     <t>ArmorPrimorite</t>
+  </si>
+  <si>
+    <t>SkillType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TargetAreaType </t>
+  </si>
+  <si>
+    <t>Wukong_FirstSkil</t>
+  </si>
+  <si>
+    <t>Wukong_SecondSkill</t>
+  </si>
+  <si>
+    <t>Wukong_ThirdSkill</t>
+  </si>
+  <si>
+    <t>Wukong_FirstSkil_Name</t>
+  </si>
+  <si>
+    <t>Wukong_SecondSkill_Name</t>
+  </si>
+  <si>
+    <t>Wukong_ThirdSkill_Name</t>
+  </si>
+  <si>
+    <t>Wukong_FirstSkil_Des</t>
+  </si>
+  <si>
+    <t>Wukong_SecondSkill_Des</t>
+  </si>
+  <si>
+    <t>Wukong_ThirdSkill_Des</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Aoe</t>
+  </si>
+  <si>
+    <t>MaxLevel</t>
+  </si>
+  <si>
+    <t>SkillID</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>CoolDown</t>
+  </si>
+  <si>
+    <t>UnlockTriggerTypes</t>
+  </si>
+  <si>
+    <t>UnlockTriggerValues</t>
+  </si>
+  <si>
+    <t>DMG_CRIT:30</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>Stackaable</t>
+  </si>
+  <si>
+    <t>MaxStack</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>DEBUFF_DEF</t>
+  </si>
+  <si>
+    <t>DEBUFF_DEF_NAME</t>
+  </si>
+  <si>
+    <t>DEBUFF_DEF_DES</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>BUFF_DEF_NAME</t>
+  </si>
+  <si>
+    <t>BUFF_DEF</t>
+  </si>
+  <si>
+    <t>BUFF_DEF_DES</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>RESIST_DEBUFF</t>
+  </si>
+  <si>
+    <t>RESIST_DEBUFF_NAME</t>
+  </si>
+  <si>
+    <t>RESIST_DEBUFF_DES</t>
+  </si>
+  <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>DEBUFF_RECEIVE</t>
+  </si>
+  <si>
+    <t>DEBUFF_RECEIVE_NAME</t>
+  </si>
+  <si>
+    <t>DEBUFF_RECEIVE_DES</t>
+  </si>
+  <si>
+    <t>DEBUFF_ATTACK</t>
+  </si>
+  <si>
+    <t>DEBUFF_ATTACK_NAME</t>
+  </si>
+  <si>
+    <t>DEBUFF_ATTACK_DES</t>
+  </si>
+  <si>
+    <t>BUFF_ATTACK</t>
+  </si>
+  <si>
+    <t>BUFF_ATTACK_NAME</t>
+  </si>
+  <si>
+    <t>BUFF_ATTACK_DES</t>
+  </si>
+  <si>
+    <t>DEBUFF_HEAL</t>
+  </si>
+  <si>
+    <t>DEBUFF_HEAL_NAME</t>
+  </si>
+  <si>
+    <t>DEBUFF_HEAL_DES</t>
+  </si>
+  <si>
+    <t>DEBUFF_STUN</t>
+  </si>
+  <si>
+    <t>DEBUFF_STUN_NAME</t>
+  </si>
+  <si>
+    <t>DEBUFF_STUN_DES</t>
+  </si>
+  <si>
+    <t>Character_ID</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>Trigger_Type</t>
+  </si>
+  <si>
+    <t>Passives</t>
+  </si>
+  <si>
+    <t>Effects</t>
+  </si>
+  <si>
+    <t>Healing_Proc:30</t>
+  </si>
+  <si>
+    <t>DEBUFF_DEF:70</t>
+  </si>
+  <si>
+    <t>CountDown</t>
+  </si>
+  <si>
+    <t>Cooldown</t>
+  </si>
+  <si>
+    <t>Wukong_FirstSkil_P1</t>
+  </si>
+  <si>
+    <t>Wukong_FirstSkil_P2</t>
+  </si>
+  <si>
+    <t>Wukong_FirstSkil_P3</t>
+  </si>
+  <si>
+    <t>CRIT_DAMGE</t>
+  </si>
+  <si>
+    <t>Taget</t>
+  </si>
+  <si>
+    <t>DMG_CRIT</t>
+  </si>
+  <si>
+    <t>Wukong_SecondSkill_P1</t>
+  </si>
+  <si>
+    <t>Wukong_SecondSkill_P2</t>
+  </si>
+  <si>
+    <t>Wukong_SecondSkill_P3</t>
+  </si>
+  <si>
+    <t>Wukong_ThirdSkill_P1</t>
+  </si>
+  <si>
+    <t>Wukong_ThirdSkill_P2</t>
+  </si>
+  <si>
+    <t>Wukong_ThirdSkill_P3</t>
+  </si>
+  <si>
+    <t>STR_ST_SKIL_DES</t>
+  </si>
+  <si>
+    <t>STR_CRIT_COOLDOWN_ULTIMATE</t>
+  </si>
+  <si>
+    <t>STR_DMG_CRIT</t>
+  </si>
+  <si>
+    <t>STR_SKILL_COOLDOWN</t>
+  </si>
+  <si>
+    <t>CRIT_COOL_DOWN_ULTIMATE:1</t>
+  </si>
+  <si>
+    <t>CRIT_COOL_DOWN_ULTIMATE</t>
+  </si>
+  <si>
+    <t>STR_RESIST_DEFBUFF</t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1208,6 +1452,9 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1493,7 +1740,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1995,7 +2242,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2170,7 +2417,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2867,7 +3114,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3293,6 +3540,728 @@
       </c>
       <c r="L11" s="14">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="5" customWidth="1"/>
+    <col min="8" max="9" width="12" style="5" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>389</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>337</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>338</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>390</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>397</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>351</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>392</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="G2" s="5">
+        <v>60</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>340</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="C3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D3" t="s">
+        <v>346</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="G3" s="5">
+        <v>60</v>
+      </c>
+      <c r="H3" s="5">
+        <v>4</v>
+      </c>
+      <c r="I3" s="5">
+        <v>4</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>341</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="C4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D4" t="s">
+        <v>347</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="G4" s="5">
+        <v>160</v>
+      </c>
+      <c r="H4" s="5">
+        <v>5</v>
+      </c>
+      <c r="I4" s="5">
+        <v>4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>395</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17" style="5" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>352</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>352</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>356</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>390</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>396</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>393</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5">
+        <v>90</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="D3" s="5">
+        <v>5</v>
+      </c>
+      <c r="E3" s="5">
+        <v>90</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>400</v>
+      </c>
+      <c r="B4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="D4" s="5">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5">
+        <v>90</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>357</v>
+      </c>
+      <c r="I4" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>404</v>
+      </c>
+      <c r="B5" t="s">
+        <v>340</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5">
+        <v>80</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>405</v>
+      </c>
+      <c r="B6" t="s">
+        <v>340</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="D6" s="5">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5">
+        <v>80</v>
+      </c>
+      <c r="F6" s="5">
+        <v>-1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>406</v>
+      </c>
+      <c r="B7" t="s">
+        <v>340</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="D7" s="5">
+        <v>9</v>
+      </c>
+      <c r="E7" s="5">
+        <v>100</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>407</v>
+      </c>
+      <c r="B8" t="s">
+        <v>341</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="D8" s="5">
+        <v>4</v>
+      </c>
+      <c r="E8" s="5">
+        <v>200</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>408</v>
+      </c>
+      <c r="B9" t="s">
+        <v>341</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="D9" s="5">
+        <v>7</v>
+      </c>
+      <c r="E9" s="5">
+        <v>200</v>
+      </c>
+      <c r="F9" s="5">
+        <v>-1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>409</v>
+      </c>
+      <c r="B10" t="s">
+        <v>341</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="D10" s="5">
+        <v>10</v>
+      </c>
+      <c r="E10" s="5">
+        <v>200</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>370</v>
+      </c>
+      <c r="I10" t="s">
+        <v>416</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="3" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>358</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>359</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D2" t="s">
+        <v>365</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5">
+        <v>2</v>
+      </c>
+      <c r="H2" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C3" t="s">
+        <v>368</v>
+      </c>
+      <c r="D3" t="s">
+        <v>369</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>370</v>
+      </c>
+      <c r="B4" t="s">
+        <v>371</v>
+      </c>
+      <c r="C4" t="s">
+        <v>372</v>
+      </c>
+      <c r="D4" t="s">
+        <v>373</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>374</v>
+      </c>
+      <c r="B5" t="s">
+        <v>375</v>
+      </c>
+      <c r="C5" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5" t="s">
+        <v>365</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>377</v>
+      </c>
+      <c r="B6" t="s">
+        <v>378</v>
+      </c>
+      <c r="C6" t="s">
+        <v>379</v>
+      </c>
+      <c r="D6" t="s">
+        <v>365</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5">
+        <v>2</v>
+      </c>
+      <c r="H6" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>380</v>
+      </c>
+      <c r="B7" t="s">
+        <v>381</v>
+      </c>
+      <c r="C7" t="s">
+        <v>382</v>
+      </c>
+      <c r="D7" t="s">
+        <v>369</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5">
+        <v>2</v>
+      </c>
+      <c r="H7" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>383</v>
+      </c>
+      <c r="B8" t="s">
+        <v>384</v>
+      </c>
+      <c r="C8" t="s">
+        <v>385</v>
+      </c>
+      <c r="D8" t="s">
+        <v>365</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>386</v>
+      </c>
+      <c r="B9" t="s">
+        <v>387</v>
+      </c>
+      <c r="C9" t="s">
+        <v>388</v>
+      </c>
+      <c r="D9" t="s">
+        <v>365</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>391</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>403</v>
+      </c>
+      <c r="B3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -3503,8 +4472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3512,6 +4481,7 @@
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
+ Clean Code and data. Create the Sprite Atlas.
</commit_message>
<xml_diff>
--- a/Assets/Data/GameConfig.xlsx
+++ b/Assets/Data/GameConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="8" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="7" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon" sheetId="4" r:id="rId1"/>
@@ -2242,7 +2242,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2417,7 +2417,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2697,7 +2697,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3706,7 +3706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -4220,8 +4220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5215,7 +5215,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C2" sqref="C2:D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>